<commit_message>
add argparse in main
</commit_message>
<xml_diff>
--- a/i2up/excel/samples.xlsx
+++ b/i2up/excel/samples.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sun_xo/learn/py/i2up/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228D3803-DAF7-E648-A752-2012B02A2F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9E6489-DA20-0549-80B5-8D6CC23E90A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="520" windowWidth="28140" windowHeight="15180" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28880" yWindow="3300" windowWidth="28140" windowHeight="15180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="work_node" sheetId="7" r:id="rId1"/>
-    <sheet name="db_node" sheetId="9" r:id="rId2"/>
+    <sheet name="msq_node" sheetId="9" r:id="rId2"/>
     <sheet name="kfk_node" sheetId="10" r:id="rId3"/>
     <sheet name="msq_msq_rule" sheetId="8" r:id="rId4"/>
     <sheet name="msq_kfk_rule" sheetId="11" r:id="rId5"/>
@@ -980,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C49F8E9-B962-1843-8F78-FE23AAE2A24E}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1432,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F785585-F36B-294D-B818-49D5E8C12014}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
add hbase-hbase rule to i2up
</commit_message>
<xml_diff>
--- a/i2up/excel/samples.xlsx
+++ b/i2up/excel/samples.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sun_xo/learn/py/i2up/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9E6489-DA20-0549-80B5-8D6CC23E90A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFC4309-EB59-2049-9717-418437531C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28880" yWindow="3300" windowWidth="28140" windowHeight="15180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32280" yWindow="1480" windowWidth="28140" windowHeight="15180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="work_node" sheetId="7" r:id="rId1"/>
     <sheet name="msq_node" sheetId="9" r:id="rId2"/>
-    <sheet name="kfk_node" sheetId="10" r:id="rId3"/>
-    <sheet name="msq_msq_rule" sheetId="8" r:id="rId4"/>
-    <sheet name="msq_kfk_rule" sheetId="11" r:id="rId5"/>
+    <sheet name="hb_node" sheetId="12" r:id="rId3"/>
+    <sheet name="kfk_node" sheetId="10" r:id="rId4"/>
+    <sheet name="msq_msq_rule" sheetId="8" r:id="rId5"/>
+    <sheet name="msq_kfk_rule" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="82">
   <si>
     <t>msq_u_auto</t>
   </si>
@@ -475,6 +476,30 @@
   </si>
   <si>
     <t>源库|备库</t>
+  </si>
+  <si>
+    <t>/hbase</t>
+  </si>
+  <si>
+    <t>hbase</t>
+  </si>
+  <si>
+    <t>zk端口</t>
+  </si>
+  <si>
+    <t>zk节点</t>
+  </si>
+  <si>
+    <t>zkIP</t>
+  </si>
+  <si>
+    <t>hb_u</t>
+  </si>
+  <si>
+    <t>hb_c2</t>
+  </si>
+  <si>
+    <t>192.168.55.12</t>
   </si>
 </sst>
 </file>
@@ -980,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C49F8E9-B962-1843-8F78-FE23AAE2A24E}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1114,6 +1139,143 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1505F4D5-7932-7941-8F0B-447A680F701D}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12:F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5">
+        <v>8020</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="5">
+        <v>2181</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="5">
+        <v>8020</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" s="5">
+        <v>2181</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A00E08A5-ABC4-3947-A76D-AB94C6311FFD}">
   <dimension ref="A1:L15"/>
   <sheetViews>
@@ -1214,7 +1376,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C76AAA83-80DE-C04C-95F4-C95AE871C727}">
   <dimension ref="A1:S5"/>
   <sheetViews>
@@ -1428,7 +1590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F785585-F36B-294D-B818-49D5E8C12014}">
   <dimension ref="A1:P4"/>
   <sheetViews>

</xml_diff>